<commit_message>
Actualización desde MV -datos-
</commit_message>
<xml_diff>
--- a/Banco Central/3/1/Tasa de política monetaria y de la facilidad permanente 2021 - Diaria.xlsx
+++ b/Banco Central/3/1/Tasa de política monetaria y de la facilidad permanente 2021 - Diaria.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t>Serie</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>04-08-2021</t>
+  </si>
+  <si>
+    <t>05-08-2021</t>
   </si>
 </sst>
 </file>
@@ -827,7 +830,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2919,6 +2922,14 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>152</v>
+      </c>
+      <c r="B150">
+        <v>0.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>